<commit_message>
adicionando as duas palestras mais recentes
</commit_message>
<xml_diff>
--- a/data/raw data/19abr2017.xlsx
+++ b/data/raw data/19abr2017.xlsx
@@ -96,9 +96,6 @@
     <t>Inseto-Planta</t>
   </si>
   <si>
-    <t>Rafael Lira T Santos</t>
-  </si>
-  <si>
     <t>Graduacao</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>Peixes</t>
   </si>
   <si>
-    <t>Yuri de Castro Azevedo</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>Lucas da Silva</t>
   </si>
   <si>
-    <t>Beaztriz Lemos Adelino</t>
-  </si>
-  <si>
     <t>David Gelcer</t>
   </si>
   <si>
@@ -172,6 +163,15 @@
   </si>
   <si>
     <t>Mes</t>
+  </si>
+  <si>
+    <t>Beatriz Lemos Adelino</t>
+  </si>
+  <si>
+    <t>Rafael Lira Teixeira Santos</t>
+  </si>
+  <si>
+    <t>Yuri Azevedo</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -533,7 +533,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -542,7 +542,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -732,13 +732,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -784,16 +784,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
@@ -836,13 +836,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
@@ -862,19 +862,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F14" s="1">
         <v>19</v>
@@ -888,19 +888,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F15" s="1">
         <v>19</v>
@@ -914,19 +914,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F16" s="1">
         <v>19</v>
@@ -940,19 +940,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F17" s="1">
         <v>19</v>
@@ -966,13 +966,13 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
@@ -992,13 +992,13 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
@@ -1018,19 +1018,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" s="1">
         <v>19</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
@@ -1056,7 +1056,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F21" s="1">
         <v>19</v>

</xml_diff>